<commit_message>
Implemented loading of equipment and related exercises into the database
</commit_message>
<xml_diff>
--- a/Equipment.xlsx
+++ b/Equipment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\College\Johns Hopkins University\compsci\autonomic-computing\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmoga\Documents\GitHub\autonomic-gym\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1007EB39-F13C-464A-A532-5716795FAA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB950F13-BEA9-4F3E-82E5-9EF59B77DB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{484F6B9E-08FA-427D-9A44-E9319AC3AAE8}"/>
+    <workbookView xWindow="28680" yWindow="585" windowWidth="29040" windowHeight="15720" xr2:uid="{484F6B9E-08FA-427D-9A44-E9319AC3AAE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
-  <si>
-    <t>smith_machine_1</t>
-  </si>
-  <si>
-    <t>smith_machine_2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
   <si>
     <t>plate_loaded_shoulder_press</t>
   </si>
@@ -68,9 +62,6 @@
     <t>hack_squat_2</t>
   </si>
   <si>
-    <t>plate_loaded_chest_press</t>
-  </si>
-  <si>
     <t>machine_leg_extension_1</t>
   </si>
   <si>
@@ -155,9 +146,6 @@
     <t>workouts</t>
   </si>
   <si>
-    <t>Smith Machine</t>
-  </si>
-  <si>
     <t>Hack Squat</t>
   </si>
   <si>
@@ -182,9 +170,6 @@
     <t>Plate Loaded Calf Press</t>
   </si>
   <si>
-    <t>Plate Loaded Chest Press</t>
-  </si>
-  <si>
     <t>Machine Incline Chest Press</t>
   </si>
   <si>
@@ -321,6 +306,9 @@
   </si>
   <si>
     <t>["Rear Delt Fly", "Reverse Flyes", "Chest Flyes"]</t>
+  </si>
+  <si>
+    <t>["Machine Shoulder (Military) Press"]</t>
   </si>
 </sst>
 </file>
@@ -701,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284DEA13-5169-41B3-99FA-5C6ABB093E17}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,16 +705,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -734,10 +722,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -745,10 +736,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -756,13 +750,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -770,69 +764,69 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,13 +834,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,13 +848,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -868,10 +862,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,13 +876,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,13 +890,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,13 +904,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,13 +918,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -935,13 +932,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -949,13 +946,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -963,13 +960,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -977,13 +974,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -991,13 +988,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,77 +1002,83 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>88</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1083,13 +1086,13 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,13 +1100,13 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,13 +1114,13 @@
         <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,13 +1128,13 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="D31" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,13 +1142,13 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1153,13 +1156,13 @@
         <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,13 +1170,13 @@
         <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1181,13 +1184,13 @@
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1195,55 +1198,13 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>